<commit_message>
dev environment 20220929 1430
</commit_message>
<xml_diff>
--- a/Tickets/Normal Tickets/Ticket 31462/Test Plan.xlsx
+++ b/Tickets/Normal Tickets/Ticket 31462/Test Plan.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin's Work\Tickets\Normal Tickets\Ticket 31462\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\WIP\Tickets\Normal Tickets\Ticket 31462\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF17FF-8F5E-4C49-9303-26ACB604BD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C7DEE-25E3-419F-8F00-BD890AD08482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31320" yWindow="780" windowWidth="24375" windowHeight="13455" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="40" r:id="rId1"/>
     <sheet name="Case #1" sheetId="33" r:id="rId2"/>
+    <sheet name="Case #2" sheetId="41" r:id="rId3"/>
+    <sheet name="Case #3" sheetId="42" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Case #1'!$1:$5</definedName>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="139">
   <si>
     <t>Test Case #</t>
   </si>
@@ -131,9 +133,6 @@
     <t>Access to SugarCRM</t>
   </si>
   <si>
-    <t>Justin Pope - 9/13/2022</t>
-  </si>
-  <si>
     <t>Test adding email to system tables and using procedure to send it</t>
   </si>
   <si>
@@ -366,12 +365,105 @@
   </si>
   <si>
     <t xml:space="preserve">attach_query_result_as_file </t>
+  </si>
+  <si>
+    <t>Test Uniters_ErrorEmail</t>
+  </si>
+  <si>
+    <t>Justin Pope - 9/29/2022</t>
+  </si>
+  <si>
+    <t>Stage records</t>
+  </si>
+  <si>
+    <t>PK_ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Policy Type</t>
+  </si>
+  <si>
+    <t>Policy Exact</t>
+  </si>
+  <si>
+    <t>Date Transmitted</t>
+  </si>
+  <si>
+    <t>Response Code</t>
+  </si>
+  <si>
+    <t>Response Text</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>304-1010579</t>
+  </si>
+  <si>
+    <t>304-1023035</t>
+  </si>
+  <si>
+    <t>OUTDOOR</t>
+  </si>
+  <si>
+    <t>UOUT10</t>
+  </si>
+  <si>
+    <t>313-1000612</t>
+  </si>
+  <si>
+    <t>313-1001192</t>
+  </si>
+  <si>
+    <t>INDOOR</t>
+  </si>
+  <si>
+    <t>UIND10</t>
+  </si>
+  <si>
+    <t>{"code":"2014","message":"No items"}</t>
+  </si>
+  <si>
+    <t>Sales Order</t>
+  </si>
+  <si>
+    <t>Test WellsFargo.BuildFile</t>
+  </si>
+  <si>
+    <t>On Dev Environment, stage error responses, excute procedure, verify email</t>
+  </si>
+  <si>
+    <t>On Dev Environment, update records to trigger email, verify email</t>
+  </si>
+  <si>
+    <t>execute procedure</t>
+  </si>
+  <si>
+    <t>verify email sent</t>
+  </si>
+  <si>
+    <t>Screen shot of email</t>
+  </si>
+  <si>
+    <t>execute WellsFargo.BuildFile</t>
+  </si>
+  <si>
+    <t>This is the record is the condition the email to be sent out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -560,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -631,71 +723,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -711,13 +749,103 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="47" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,6 +901,192 @@
         <a:xfrm>
           <a:off x="95250" y="2686050"/>
           <a:ext cx="8007762" cy="3568883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4430662</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>105174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5E08E24-F26F-E11F-1C33-A44249E55D23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="2524125"/>
+          <a:ext cx="11012437" cy="2857899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>791604</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>58220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB060B06-3EBC-2733-9204-F23339139E2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="9163050"/>
+          <a:ext cx="7373379" cy="7668695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>363770</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>29401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DDA262F-C468-151C-19A0-C3A6F7782FBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="447675" y="2952750"/>
+          <a:ext cx="13041545" cy="5915851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4868773</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>9933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCC8615A-F74B-4BA3-C443-ED8E2226C736}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="9486900"/>
+          <a:ext cx="10736173" cy="2924583"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1105,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1142,148 +1456,178 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="3" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="24"/>
+    </row>
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+    </row>
+    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>1</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-    </row>
-    <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>2</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
+        <v>1</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="15" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>2</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
         <v>3</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1297,9 +1641,9 @@
   </sheetPr>
   <dimension ref="A1:AC51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q53" sqref="Q53"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1335,59 +1679,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="26">
+      <c r="B2" s="54"/>
+      <c r="C2" s="42">
         <f>'Test Cases'!A2</f>
         <v>1</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="26" t="str">
+      <c r="B3" s="54"/>
+      <c r="C3" s="42" t="str">
         <f>'Test Cases'!B2</f>
         <v>Test adding email to system tables and using procedure to send it</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="26" t="str">
+      <c r="B4" s="54"/>
+      <c r="C4" s="42" t="str">
         <f>'Test Cases'!D2</f>
         <v>1) Access to SQL08 to execute procedures</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="17" t="s">
         <v>19</v>
       </c>
@@ -1399,48 +1743,48 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
     </row>
     <row r="7" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35">
+      <c r="A7" s="57">
         <v>1</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39">
+      <c r="A9" s="49">
         <v>1</v>
       </c>
-      <c r="B9" s="40"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="13" t="s">
         <v>28</v>
       </c>
@@ -1449,10 +1793,10 @@
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39">
+      <c r="A10" s="49">
         <v>2</v>
       </c>
-      <c r="B10" s="40"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1465,10 +1809,10 @@
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41">
+      <c r="A11" s="51">
         <v>3</v>
       </c>
-      <c r="B11" s="42"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="20" t="s">
         <v>30</v>
       </c>
@@ -1477,411 +1821,406 @@
       <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45"/>
-    </row>
-    <row r="37" spans="1:29" s="50" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-    </row>
-    <row r="38" spans="1:29" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="50" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+    </row>
+    <row r="37" spans="1:29" s="32" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+    </row>
+    <row r="38" spans="1:29" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="E38" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="50" t="s">
+      <c r="F38" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="G38" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="G38" s="50" t="s">
+      <c r="H38" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H38" s="50" t="s">
+      <c r="I38" s="32" t="s">
         <v>49</v>
-      </c>
-      <c r="I38" s="50" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="E39" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="I39" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+    </row>
+    <row r="42" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K42" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="L42" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="M42" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="N42" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="O42" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="P42" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q42" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="R42" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="S42" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="U42" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="V42" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="W42" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="X42" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J43" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="L43" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="N43" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="O43" s="28">
+        <v>0</v>
+      </c>
+      <c r="P43" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="R43" s="28">
+        <v>256</v>
+      </c>
+      <c r="S43" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="T43" s="28">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28">
+        <v>0</v>
+      </c>
+      <c r="V43" s="28">
+        <v>1</v>
+      </c>
+      <c r="W43" s="28">
+        <v>0</v>
+      </c>
+      <c r="X43" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D44" s="29"/>
+    </row>
+    <row r="45" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-    </row>
-    <row r="42" spans="1:29" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G42" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="H42" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="I42" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="J42" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="K42" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="L42" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="M42" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="N42" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="O42" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="P42" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q42" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="R42" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="S42" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="T42" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="U42" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="V42" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="W42" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="X42" s="48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" s="46" t="s">
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+    </row>
+    <row r="46" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I46" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="K46" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="L46" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M46" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="N46" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="O46" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="P46" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q46" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="R46" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="S46" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="T46" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="U46" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="V46" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="W46" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="X46" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y46" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z46" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA46" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB46" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC46" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="28">
+        <v>158146</v>
+      </c>
+      <c r="D47" s="29">
+        <v>2</v>
+      </c>
+      <c r="E47" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="46" t="s">
+      <c r="F47" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="H43" s="46" t="s">
+      <c r="I47" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="J47" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="J43" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="K43" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="L43" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="M43" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N43" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="O43" s="46">
+      <c r="K47" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L47" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="N47" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O47" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="P47" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q47" s="28">
         <v>0</v>
       </c>
-      <c r="P43" s="46">
+      <c r="R47" s="28">
         <v>0</v>
       </c>
-      <c r="Q43" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="R43" s="46">
+      <c r="S47" s="28">
         <v>256</v>
       </c>
-      <c r="S43" s="46" t="s">
+      <c r="T47" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="T43" s="46">
+      <c r="U47" s="28">
         <v>0</v>
       </c>
-      <c r="U43" s="46">
+      <c r="V47" s="28">
         <v>0</v>
       </c>
-      <c r="V43" s="46">
-        <v>1</v>
-      </c>
-      <c r="W43" s="46">
-        <v>0</v>
-      </c>
-      <c r="X43" s="46" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="47"/>
-    </row>
-    <row r="45" spans="1:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-    </row>
-    <row r="46" spans="1:29" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F46" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="G46" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="H46" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="I46" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="J46" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="K46" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="L46" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="M46" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="N46" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="O46" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="P46" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q46" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="R46" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="S46" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="T46" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="U46" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="V46" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="W46" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="X46" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y46" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z46" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA46" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB46" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC46" s="48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="46">
-        <v>158146</v>
-      </c>
-      <c r="D47" s="47">
-        <v>2</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="H47" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="I47" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="J47" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="K47" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="L47" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="M47" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="N47" s="46" t="s">
+      <c r="W47" s="34">
+        <v>44816.499597569447</v>
+      </c>
+      <c r="X47" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="O47" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="P47" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q47" s="46">
-        <v>0</v>
-      </c>
-      <c r="R47" s="46">
-        <v>0</v>
-      </c>
-      <c r="S47" s="46">
-        <v>256</v>
-      </c>
-      <c r="T47" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="U47" s="46">
-        <v>0</v>
-      </c>
-      <c r="V47" s="46">
-        <v>0</v>
-      </c>
-      <c r="W47" s="54">
-        <v>44816.499597569447</v>
-      </c>
-      <c r="X47" s="46" t="s">
+      <c r="Y47" s="28">
+        <v>4</v>
+      </c>
+      <c r="Z47" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="Y47" s="46">
-        <v>4</v>
-      </c>
-      <c r="Z47" s="46" t="s">
+      <c r="AA47" s="34">
+        <v>44816.499594907407</v>
+      </c>
+      <c r="AB47" s="34">
+        <v>44816.499601886571</v>
+      </c>
+      <c r="AC47" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="AA47" s="54">
-        <v>44816.499594907407</v>
-      </c>
-      <c r="AB47" s="54">
-        <v>44816.499601886571</v>
-      </c>
-      <c r="AC47" s="46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="47"/>
-    </row>
-    <row r="49" spans="4:4" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="47"/>
-    </row>
-    <row r="50" spans="4:4" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="47"/>
-    </row>
-    <row r="51" spans="4:4" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="47"/>
+    </row>
+    <row r="48" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="29"/>
+    </row>
+    <row r="49" spans="4:4" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D49" s="29"/>
+    </row>
+    <row r="50" spans="4:4" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D50" s="29"/>
+    </row>
+    <row r="51" spans="4:4" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A1:E1"/>
@@ -1895,6 +2234,11 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1904,22 +2248,1210 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEC7422-07D1-4D64-93C0-A640E08B2D7B}">
+  <dimension ref="A1:AB52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="96.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="60" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="53"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="42">
+        <f>'Test Cases'!A3</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="42" t="str">
+        <f>'Test Cases'!B3</f>
+        <v>Test Uniters_ErrorEmail</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="42" t="str">
+        <f>'Test Cases'!D3</f>
+        <v>1) Access to SQL08 to execute procedures</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="57">
+        <v>1</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+    </row>
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+    </row>
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49">
+        <v>1</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+    </row>
+    <row r="31" spans="2:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="J31" s="62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="62">
+        <v>3466</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="64">
+        <v>44832.649260416663</v>
+      </c>
+      <c r="I32" s="62">
+        <v>12029</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="62">
+        <v>3474</v>
+      </c>
+      <c r="C33" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I33" s="62">
+        <v>400</v>
+      </c>
+      <c r="J33" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="62">
+        <v>3475</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H34" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I34" s="62">
+        <v>400</v>
+      </c>
+      <c r="J34" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="62">
+        <v>3476</v>
+      </c>
+      <c r="C35" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I35" s="62">
+        <v>400</v>
+      </c>
+      <c r="J35" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" s="62" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="62">
+        <v>3477</v>
+      </c>
+      <c r="C36" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F36" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I36" s="62">
+        <v>400</v>
+      </c>
+      <c r="J36" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="62">
+        <v>3478</v>
+      </c>
+      <c r="C37" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I37" s="62">
+        <v>400</v>
+      </c>
+      <c r="J37" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="62">
+        <v>3479</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H38" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I38" s="62">
+        <v>400</v>
+      </c>
+      <c r="J38" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="62">
+        <v>3480</v>
+      </c>
+      <c r="C39" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I39" s="62">
+        <v>400</v>
+      </c>
+      <c r="J39" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="2:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="62">
+        <v>3481</v>
+      </c>
+      <c r="C40" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I40" s="62">
+        <v>400</v>
+      </c>
+      <c r="J40" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="65">
+        <v>3482</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I41" s="65">
+        <v>400</v>
+      </c>
+      <c r="J41" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="65">
+        <v>3483</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I42" s="65">
+        <v>400</v>
+      </c>
+      <c r="J42" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="65">
+        <v>3484</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G43" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I43" s="65">
+        <v>400</v>
+      </c>
+      <c r="J43" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="65">
+        <v>3485</v>
+      </c>
+      <c r="C44" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D44" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G44" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I44" s="65">
+        <v>400</v>
+      </c>
+      <c r="J44" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="65">
+        <v>3486</v>
+      </c>
+      <c r="C45" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G45" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H45" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I45" s="65">
+        <v>400</v>
+      </c>
+      <c r="J45" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="65">
+        <v>3487</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I46" s="65">
+        <v>400</v>
+      </c>
+      <c r="J46" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="W46" s="68"/>
+      <c r="AA46" s="68"/>
+      <c r="AB46" s="68"/>
+    </row>
+    <row r="47" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="65">
+        <v>3488</v>
+      </c>
+      <c r="C47" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G47" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H47" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I47" s="65">
+        <v>400</v>
+      </c>
+      <c r="J47" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="65">
+        <v>3489</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G48" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I48" s="65">
+        <v>400</v>
+      </c>
+      <c r="J48" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="65">
+        <v>3490</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G49" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H49" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I49" s="65">
+        <v>400</v>
+      </c>
+      <c r="J49" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="65">
+        <v>3491</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H50" s="67">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I50" s="65">
+        <v>400</v>
+      </c>
+      <c r="J50" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="62">
+        <v>3492</v>
+      </c>
+      <c r="C51" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H51" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I51" s="62">
+        <v>400</v>
+      </c>
+      <c r="J51" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="62">
+        <v>3493</v>
+      </c>
+      <c r="C52" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="F52" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="H52" s="64">
+        <v>44832.659401122684</v>
+      </c>
+      <c r="I52" s="62">
+        <v>400</v>
+      </c>
+      <c r="J52" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a638d2c-e7c0-419c-9191-e92086f67d97">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="84e25877-5f26-4dc3-9598-48e40fb4ec5c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE81EED-E8A6-4F0F-A183-D91B3AA18A59}">
+  <dimension ref="A1:AB53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="96.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="60" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="53"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="42">
+        <f>'Test Cases'!A4</f>
+        <v>3</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="42" t="str">
+        <f>'Test Cases'!B4</f>
+        <v>Test WellsFargo.BuildFile</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="42" t="str">
+        <f>'Test Cases'!D4</f>
+        <v>1) Access to SQL08 to execute procedures</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="57">
+        <v>1</v>
+      </c>
+      <c r="B7" s="58"/>
+      <c r="C7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="57">
+        <v>2</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+    </row>
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="57">
+        <v>3</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+    </row>
+    <row r="10" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49">
+        <v>1</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+    </row>
+    <row r="12" spans="1:8" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+    </row>
+    <row r="14" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="63"/>
+      <c r="H32" s="64"/>
+    </row>
+    <row r="33" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D33" s="63"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+    </row>
+    <row r="34" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="63"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+    </row>
+    <row r="35" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="63"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+    </row>
+    <row r="36" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="63"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+    </row>
+    <row r="37" spans="4:28" s="62" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+    </row>
+    <row r="38" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="63"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+    </row>
+    <row r="39" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="63"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+    </row>
+    <row r="40" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D40" s="63"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+    </row>
+    <row r="41" spans="4:28" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+    </row>
+    <row r="42" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D42" s="66"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+    </row>
+    <row r="43" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D43" s="66"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+    </row>
+    <row r="44" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D44" s="66"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+    </row>
+    <row r="45" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+    </row>
+    <row r="46" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D46" s="66"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+    </row>
+    <row r="47" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D47" s="66"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="W47" s="68"/>
+      <c r="AA47" s="68"/>
+      <c r="AB47" s="68"/>
+    </row>
+    <row r="48" spans="4:28" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="66"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+    </row>
+    <row r="49" spans="4:8" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D49" s="66"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+    </row>
+    <row r="50" spans="4:8" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D50" s="66"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+    </row>
+    <row r="51" spans="4:8" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D51" s="66"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+    </row>
+    <row r="52" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D52" s="63"/>
+      <c r="G52" s="64"/>
+      <c r="H52" s="64"/>
+    </row>
+    <row r="53" spans="4:8" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D53" s="63"/>
+      <c r="G53" s="64"/>
+      <c r="H53" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C2685AC3E5C784C94699E6BCD3719C2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc4032ed2b9525712665d7b053f58e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a638d2c-e7c0-419c-9191-e92086f67d97" xmlns:ns3="84e25877-5f26-4dc3-9598-48e40fb4ec5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60642ebedafdd5f29702615754875760" ns2:_="" ns3:_="">
     <xsd:import namespace="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
@@ -2150,6 +3682,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a638d2c-e7c0-419c-9191-e92086f67d97">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="84e25877-5f26-4dc3-9598-48e40fb4ec5c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2160,25 +3707,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D54ED65-933A-4F90-B95A-15C952E0CAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E225A3-DBF5-416D-8482-D016D280651E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2197,6 +3725,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D54ED65-933A-4F90-B95A-15C952E0CAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
   <ds:schemaRefs>

</xml_diff>